<commit_message>
Add : knn using sklearn
</commit_message>
<xml_diff>
--- a/hsv.xlsx
+++ b/hsv.xlsx
@@ -11,6 +11,29 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+  <si>
+    <t>Hue</t>
+  </si>
+  <si>
+    <t>Saturation</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>apples</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,101 +363,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
         <v>75.58709790820559</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>120.8249871173414</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>201.17367155771</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
         <v>82.909043</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>102.062282</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>198.609373</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>53.38122845691382</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>86.21186072144289</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>222.1369839679359</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>65.33967407407407</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>74.80638024691358</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>238.7269925925926</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>52.48621255547337</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>79.01244683801775</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>213.0833140717456</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
         <v>43.41056908417152</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>49.15904865890242</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>85.36712987471326</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
         <v>51.4495420856347</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>85.15149884341217</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>215.4209401406789</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>55.548436</v>
-      </c>
-      <c r="B8">
-        <v>71.925392</v>
-      </c>
-      <c r="C8">
-        <v>219.5243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>70.18737704918033</v>
       </c>
@@ -444,8 +491,11 @@
       <c r="C9">
         <v>246.5066084189035</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>65.96455498312311</v>
       </c>
@@ -455,82 +505,78 @@
       <c r="C10">
         <v>248.8740765085569</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
-        <v>43.51049858109956</v>
+        <v>59.88201152852316</v>
       </c>
       <c r="B11">
-        <v>91.97278446389497</v>
+        <v>110.7303319419598</v>
       </c>
       <c r="C11">
-        <v>240.5210698167396</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>234.7669846948917</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
-        <v>59.88201152852316</v>
+        <v>48.4713381723432</v>
       </c>
       <c r="B12">
-        <v>110.7303319419598</v>
+        <v>91.38520147031454</v>
       </c>
       <c r="C12">
-        <v>234.7669846948917</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>246.4205983621813</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
-        <v>48.4713381723432</v>
+        <v>76.21333333333334</v>
       </c>
       <c r="B13">
-        <v>91.38520147031454</v>
+        <v>129.8308938271605</v>
       </c>
       <c r="C13">
-        <v>246.4205983621813</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>241.6286222222222</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
-        <v>76.21333333333334</v>
+        <v>53.865828</v>
       </c>
       <c r="B14">
-        <v>129.8308938271605</v>
+        <v>93.35978</v>
       </c>
       <c r="C14">
-        <v>241.6286222222222</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>239.147624</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
-        <v>53.865828</v>
+        <v>53.64759370314842</v>
       </c>
       <c r="B15">
-        <v>93.35978</v>
+        <v>62.83002098950525</v>
       </c>
       <c r="C15">
-        <v>239.147624</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>53.64759370314842</v>
-      </c>
-      <c r="B16">
-        <v>62.83002098950525</v>
-      </c>
-      <c r="C16">
         <v>249.6973043478261</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>45.16696981424148</v>
-      </c>
-      <c r="B17">
-        <v>88.71430147058824</v>
-      </c>
-      <c r="C17">
-        <v>253.3402476780186</v>
+      <c r="D15" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Init : knn that don't use sklearn
</commit_message>
<xml_diff>
--- a/hsv.xlsx
+++ b/hsv.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
   <si>
     <t>Hue</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Class</t>
   </si>
   <si>
-    <t>apples</t>
+    <t>apple</t>
   </si>
   <si>
     <t>orange</t>
@@ -363,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -469,13 +469,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>51.4495420856347</v>
+        <v>50.84785917930964</v>
       </c>
       <c r="B8">
-        <v>85.15149884341217</v>
+        <v>68.93794165563588</v>
       </c>
       <c r="C8">
-        <v>215.4209401406789</v>
+        <v>208.8774615619591</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -483,27 +483,27 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>70.18737704918033</v>
+        <v>51.4495420856347</v>
       </c>
       <c r="B9">
-        <v>145.4080423947637</v>
+        <v>85.15149884341217</v>
       </c>
       <c r="C9">
-        <v>246.5066084189035</v>
+        <v>215.4209401406789</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>65.96455498312311</v>
+        <v>70.18737704918033</v>
       </c>
       <c r="B10">
-        <v>115.6808497660923</v>
+        <v>145.4080423947637</v>
       </c>
       <c r="C10">
-        <v>248.8740765085569</v>
+        <v>246.5066084189035</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -511,13 +511,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>59.88201152852316</v>
+        <v>65.96455498312311</v>
       </c>
       <c r="B11">
-        <v>110.7303319419598</v>
+        <v>115.6808497660923</v>
       </c>
       <c r="C11">
-        <v>234.7669846948917</v>
+        <v>248.8740765085569</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -525,13 +525,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>48.4713381723432</v>
+        <v>43.51049858109956</v>
       </c>
       <c r="B12">
-        <v>91.38520147031454</v>
+        <v>91.97278446389497</v>
       </c>
       <c r="C12">
-        <v>246.4205983621813</v>
+        <v>240.5210698167396</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -539,13 +539,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>76.21333333333334</v>
+        <v>59.88201152852316</v>
       </c>
       <c r="B13">
-        <v>129.8308938271605</v>
+        <v>110.7303319419598</v>
       </c>
       <c r="C13">
-        <v>241.6286222222222</v>
+        <v>234.7669846948917</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -553,13 +553,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>53.865828</v>
+        <v>48.4713381723432</v>
       </c>
       <c r="B14">
-        <v>93.35978</v>
+        <v>91.38520147031454</v>
       </c>
       <c r="C14">
-        <v>239.147624</v>
+        <v>246.4205983621813</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -567,15 +567,43 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
+        <v>76.21333333333334</v>
+      </c>
+      <c r="B15">
+        <v>129.8308938271605</v>
+      </c>
+      <c r="C15">
+        <v>241.6286222222222</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>53.865828</v>
+      </c>
+      <c r="B16">
+        <v>93.35978</v>
+      </c>
+      <c r="C16">
+        <v>239.147624</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
         <v>53.64759370314842</v>
       </c>
-      <c r="B15">
+      <c r="B17">
         <v>62.83002098950525</v>
       </c>
-      <c r="C15">
+      <c r="C17">
         <v>249.6973043478261</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add : KNN without sklearn process
</commit_message>
<xml_diff>
--- a/hsv.xlsx
+++ b/hsv.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
   <si>
     <t>Hue</t>
   </si>
@@ -363,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -497,27 +497,27 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>70.18737704918033</v>
+        <v>48.53515510204082</v>
       </c>
       <c r="B10">
-        <v>145.4080423947637</v>
+        <v>62.8087693877551</v>
       </c>
       <c r="C10">
-        <v>246.5066084189035</v>
+        <v>231.1706775510204</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>65.96455498312311</v>
+        <v>70.18737704918033</v>
       </c>
       <c r="B11">
-        <v>115.6808497660923</v>
+        <v>145.4080423947637</v>
       </c>
       <c r="C11">
-        <v>248.8740765085569</v>
+        <v>246.5066084189035</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
@@ -525,13 +525,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>43.51049858109956</v>
+        <v>65.96455498312311</v>
       </c>
       <c r="B12">
-        <v>91.97278446389497</v>
+        <v>115.6808497660923</v>
       </c>
       <c r="C12">
-        <v>240.5210698167396</v>
+        <v>248.8740765085569</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -539,13 +539,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>59.88201152852316</v>
+        <v>43.51049858109956</v>
       </c>
       <c r="B13">
-        <v>110.7303319419598</v>
+        <v>91.97278446389497</v>
       </c>
       <c r="C13">
-        <v>234.7669846948917</v>
+        <v>240.5210698167396</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -553,13 +553,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>48.4713381723432</v>
+        <v>59.88201152852316</v>
       </c>
       <c r="B14">
-        <v>91.38520147031454</v>
+        <v>110.7303319419598</v>
       </c>
       <c r="C14">
-        <v>246.4205983621813</v>
+        <v>234.7669846948917</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -567,13 +567,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>76.21333333333334</v>
+        <v>48.4713381723432</v>
       </c>
       <c r="B15">
-        <v>129.8308938271605</v>
+        <v>91.38520147031454</v>
       </c>
       <c r="C15">
-        <v>241.6286222222222</v>
+        <v>246.4205983621813</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -581,13 +581,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>53.865828</v>
+        <v>76.21333333333334</v>
       </c>
       <c r="B16">
-        <v>93.35978</v>
+        <v>129.8308938271605</v>
       </c>
       <c r="C16">
-        <v>239.147624</v>
+        <v>241.6286222222222</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -595,15 +595,29 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
+        <v>53.865828</v>
+      </c>
+      <c r="B17">
+        <v>93.35978</v>
+      </c>
+      <c r="C17">
+        <v>239.147624</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
         <v>53.64759370314842</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>62.83002098950525</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <v>249.6973043478261</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add : image cropping process
</commit_message>
<xml_diff>
--- a/hsv.xlsx
+++ b/hsv.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>Hue</t>
   </si>
@@ -363,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,13 +385,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>75.58709790820559</v>
+        <v>69.93241604436875</v>
       </c>
       <c r="B2">
-        <v>120.8249871173414</v>
+        <v>119.4631494825101</v>
       </c>
       <c r="C2">
-        <v>201.17367155771</v>
+        <v>103.8289733176121</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -399,13 +399,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>82.909043</v>
+        <v>82.135966</v>
       </c>
       <c r="B3">
-        <v>102.062282</v>
+        <v>101.873225</v>
       </c>
       <c r="C3">
-        <v>198.609373</v>
+        <v>165.679404</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -413,13 +413,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>53.38122845691382</v>
+        <v>53.71473647294589</v>
       </c>
       <c r="B4">
-        <v>86.21186072144289</v>
+        <v>91.98599298597195</v>
       </c>
       <c r="C4">
-        <v>222.1369839679359</v>
+        <v>80.75693687374749</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -427,13 +427,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>65.33967407407407</v>
+        <v>44.27289855072464</v>
       </c>
       <c r="B5">
-        <v>74.80638024691358</v>
+        <v>76.99673188405797</v>
       </c>
       <c r="C5">
-        <v>238.7269925925926</v>
+        <v>50.81751449275362</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -441,13 +441,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>52.48621255547337</v>
+        <v>60.37044938271605</v>
       </c>
       <c r="B6">
-        <v>79.01244683801775</v>
+        <v>95.15539753086419</v>
       </c>
       <c r="C6">
-        <v>213.0833140717456</v>
+        <v>107.7229037037037</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -455,13 +455,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>43.41056908417152</v>
+        <v>51.40317585059172</v>
       </c>
       <c r="B7">
-        <v>49.15904865890242</v>
+        <v>88.80160179363905</v>
       </c>
       <c r="C7">
-        <v>85.36712987471326</v>
+        <v>61.59795673076923</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -469,13 +469,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>50.84785917930964</v>
+        <v>36.287939827069</v>
       </c>
       <c r="B8">
-        <v>68.93794165563588</v>
+        <v>49.08493515087348</v>
       </c>
       <c r="C8">
-        <v>208.8774615619591</v>
+        <v>69.70464002117522</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -483,13 +483,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>51.4495420856347</v>
+        <v>48.58067661134304</v>
       </c>
       <c r="B9">
-        <v>85.15149884341217</v>
+        <v>67.88466805824254</v>
       </c>
       <c r="C9">
-        <v>215.4209401406789</v>
+        <v>69.20226809897159</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -497,13 +497,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>48.53515510204082</v>
+        <v>50.54839847991314</v>
       </c>
       <c r="B10">
-        <v>62.8087693877551</v>
+        <v>84.62199877260068</v>
       </c>
       <c r="C10">
-        <v>231.1706775510204</v>
+        <v>79.21735589859793</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -511,27 +511,27 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>70.18737704918033</v>
+        <v>42.11935714285714</v>
       </c>
       <c r="B11">
-        <v>145.4080423947637</v>
+        <v>67.00360612244899</v>
       </c>
       <c r="C11">
-        <v>246.5066084189035</v>
+        <v>59.25526122448979</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>65.96455498312311</v>
+        <v>67.29704617786585</v>
       </c>
       <c r="B12">
-        <v>115.6808497660923</v>
+        <v>149.7104719870294</v>
       </c>
       <c r="C12">
-        <v>248.8740765085569</v>
+        <v>148.304458656098</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -539,13 +539,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>43.51049858109956</v>
+        <v>56.99262331971339</v>
       </c>
       <c r="B13">
-        <v>91.97278446389497</v>
+        <v>117.9771871854089</v>
       </c>
       <c r="C13">
-        <v>240.5210698167396</v>
+        <v>121.9862924142832</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -553,13 +553,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>59.88201152852316</v>
+        <v>41.46559807508206</v>
       </c>
       <c r="B14">
-        <v>110.7303319419598</v>
+        <v>95.64466373769146</v>
       </c>
       <c r="C14">
-        <v>234.7669846948917</v>
+        <v>92.07184999829047</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -567,13 +567,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>48.4713381723432</v>
+        <v>68.76905947706159</v>
       </c>
       <c r="B15">
-        <v>91.38520147031454</v>
+        <v>149.8030241356192</v>
       </c>
       <c r="C15">
-        <v>246.4205983621813</v>
+        <v>160.8261122018964</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
@@ -581,13 +581,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>76.21333333333334</v>
+        <v>56.00113297555158</v>
       </c>
       <c r="B16">
-        <v>129.8308938271605</v>
+        <v>133.1910554561717</v>
       </c>
       <c r="C16">
-        <v>241.6286222222222</v>
+        <v>110.8894454382826</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -595,13 +595,13 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>53.865828</v>
+        <v>45.22304229480737</v>
       </c>
       <c r="B17">
-        <v>93.35978</v>
+        <v>102.5357574911595</v>
       </c>
       <c r="C17">
-        <v>239.147624</v>
+        <v>96.21698190024195</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -609,15 +609,57 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>53.64759370314842</v>
+        <v>70.89307654320987</v>
       </c>
       <c r="B18">
-        <v>62.83002098950525</v>
+        <v>148.8855901234568</v>
       </c>
       <c r="C18">
-        <v>249.6973043478261</v>
+        <v>142.4722567901235</v>
       </c>
       <c r="D18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>51.632296</v>
+      </c>
+      <c r="B19">
+        <v>101.840732</v>
+      </c>
+      <c r="C19">
+        <v>107.02792</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>53.0643125</v>
+      </c>
+      <c r="B20">
+        <v>119.5098625</v>
+      </c>
+      <c r="C20">
+        <v>107.7172609375</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>30.66874062968516</v>
+      </c>
+      <c r="B21">
+        <v>66.16414992503748</v>
+      </c>
+      <c r="C21">
+        <v>68.53306746626687</v>
+      </c>
+      <c r="D21" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>